<commit_message>
Atualização do mes de novembro
</commit_message>
<xml_diff>
--- a/intranet/assets/enfermagem/FICHA DE REMOÇÃO.xlsx
+++ b/intranet/assets/enfermagem/FICHA DE REMOÇÃO.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\16 VANLI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caroline.assis\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9746B5EB-6700-4B30-ADB9-CC091A32F8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDF5341-E331-4A57-AA02-6A9865229AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{70C91AA4-8299-470B-879E-923514225B65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{70C91AA4-8299-470B-879E-923514225B65}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Planilha1!$A$1:$C$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Planilha1!$A$1:$C$73</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Informações da equipe</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Peso: ________ kg</t>
   </si>
   <si>
-    <t>Possível Diagnostico:</t>
-  </si>
-  <si>
     <t>Parentesco:</t>
   </si>
   <si>
@@ -175,17 +172,62 @@
     <t>Assinatura e carimbo no enfermeiro solicitante: _____________________</t>
   </si>
   <si>
-    <t>OBS: E.D.A e Ultrassom enviar c/ S.A.D.A.T</t>
-  </si>
-  <si>
     <t>OBRIGATÓRIO CONSTAR NA APAC: SEM CONTRASTE</t>
+  </si>
+  <si>
+    <t>EM CASO DE CATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(    ) Registros Gerais </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(    ) Cópias de docs pessoais </t>
+  </si>
+  <si>
+    <t>(    ) TR de Covid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(    ) Ficha impressa do CROSS                               </t>
+  </si>
+  <si>
+    <t>(    ) APAC</t>
+  </si>
+  <si>
+    <t>(    ) Todos Exames laboratoriais - inclusive UREIA E CREATININA / ECG/ RX / TC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(    ) Filipeta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(    ) Checar se suspensão anticoagulante conforme orientação filipeta </t>
+  </si>
+  <si>
+    <t>OBS: E.D.A enviar c/ S.A.D.A.T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(    ) Checar se realizou tricotomia em região inguinal (bilateral) </t>
+  </si>
+  <si>
+    <t>Possível Diagnóstico:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(    ) Última Evolução de Enfermagem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(    ) Última Anotação de Enfermagem                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(    ) TODAS Prescrições Médicas CHECADAS                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(    ) Última Evolução Médica                                             </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +324,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -291,7 +347,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -596,11 +652,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -648,6 +784,54 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -657,33 +841,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -711,14 +868,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -890,15 +1047,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1685925</xdr:colOff>
+      <xdr:colOff>1704975</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>286111</xdr:rowOff>
+      <xdr:rowOff>276586</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -921,8 +1078,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28575" y="4010026"/>
-          <a:ext cx="6057900" cy="1391011"/>
+          <a:off x="47625" y="9296401"/>
+          <a:ext cx="6057900" cy="1391010"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1135,13 +1292,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>809625</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>561974</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1170,7 +1327,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="13258800"/>
+          <a:off x="0" y="12534900"/>
           <a:ext cx="561974" cy="561974"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1483,10 +1640,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,144 +1663,144 @@
       <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="47"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
     </row>
     <row r="7" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="34"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="41"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="39"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="11" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="39"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="39"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="39"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="43"/>
+      <c r="C12" s="44"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="43"/>
+      <c r="C13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="10" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
+      <c r="A14" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="52"/>
+      <c r="C14" s="53"/>
     </row>
     <row r="15" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="41"/>
     </row>
     <row r="16" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
+      <c r="A17" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="52"/>
+      <c r="C17" s="53"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="31"/>
+      <c r="A18" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="52"/>
+      <c r="C18" s="53"/>
     </row>
     <row r="19" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="41"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
@@ -1675,11 +1832,11 @@
       <c r="C26" s="16"/>
     </row>
     <row r="27" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="34"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
@@ -1744,11 +1901,11 @@
       <c r="C35" s="16"/>
     </row>
     <row r="36" spans="1:11" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="43"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="56"/>
       <c r="J36" s="6"/>
       <c r="K36" s="4"/>
     </row>
@@ -1760,11 +1917,11 @@
       <c r="K37" s="4"/>
     </row>
     <row r="38" spans="1:11" ht="21" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="48"/>
-      <c r="C38" s="49"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="62"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
@@ -1797,11 +1954,11 @@
       <c r="C45" s="16"/>
     </row>
     <row r="46" spans="1:11" ht="24" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="44" t="s">
+      <c r="A46" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="45"/>
-      <c r="C46" s="46"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="59"/>
       <c r="I46" s="5" t="s">
         <v>27</v>
       </c>
@@ -1846,23 +2003,23 @@
       <c r="J50" s="3"/>
     </row>
     <row r="51" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A51" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51" s="33"/>
-      <c r="C51" s="34"/>
-    </row>
-    <row r="52" spans="1:11" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="B52" s="51"/>
-      <c r="C52" s="52"/>
+      <c r="A51" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" s="40"/>
+      <c r="C51" s="41"/>
+    </row>
+    <row r="52" spans="1:11" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="49"/>
+      <c r="C52" s="50"/>
     </row>
     <row r="53" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I54" s="18" t="s">
         <v>24</v>
@@ -1875,27 +2032,128 @@
     </row>
     <row r="56" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A56" s="28" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="I56" s="18" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="29"/>
+      <c r="B58" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" s="31"/>
+    </row>
+    <row r="59" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59" s="64"/>
+      <c r="C59" s="65"/>
+    </row>
+    <row r="60" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="32"/>
+      <c r="B60" s="33"/>
+      <c r="C60" s="34"/>
+    </row>
+    <row r="61" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="64"/>
+      <c r="C61" s="65"/>
+    </row>
+    <row r="62" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" s="64"/>
+      <c r="C62" s="65"/>
+    </row>
+    <row r="63" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" s="64"/>
+      <c r="C63" s="65"/>
+    </row>
+    <row r="64" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="B64" s="64"/>
+      <c r="C64" s="65"/>
+    </row>
+    <row r="65" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B65" s="33"/>
+      <c r="C65" s="34"/>
+    </row>
+    <row r="66" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="B66" s="64"/>
+      <c r="C66" s="65"/>
+    </row>
+    <row r="67" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="B67" s="64"/>
+      <c r="C67" s="65"/>
+    </row>
+    <row r="68" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B68" s="33"/>
+      <c r="C68" s="34"/>
+    </row>
+    <row r="69" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B69" s="33"/>
+      <c r="C69" s="34"/>
+    </row>
+    <row r="70" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B70" s="33"/>
+      <c r="C70" s="34"/>
+    </row>
+    <row r="71" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C71" s="37"/>
+    </row>
+    <row r="72" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C72" s="37"/>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="38"/>
+      <c r="B73" s="35"/>
+      <c r="C73" s="36"/>
+    </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
+  <mergeCells count="30">
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A64:C64"/>
     <mergeCell ref="A52:C52"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A18:C18"/>
@@ -1906,6 +2164,19 @@
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:C12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="99" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>